<commit_message>
Added UtilOutputReport to testthat
 (not yet checking excel write routines).
</commit_message>
<xml_diff>
--- a/vignettes/DBMH.xlsx
+++ b/vignettes/DBMH.xlsx
@@ -17,12 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Nov/29/2018</t>
+    <t xml:space="preserve">Nov/30/2018</t>
   </si>
   <si>
     <t xml:space="preserve">Input file</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">DBMH</t>
   </si>
   <si>
-    <t xml:space="preserve">Variability estimation stMethod</t>
+    <t xml:space="preserve">Variability estimation method</t>
   </si>
   <si>
     <t xml:space="preserve">Jackknife</t>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PrGTt</t>
   </si>
   <si>
     <t xml:space="preserve">95% CI's FOMs, treatment difference, each reader</t>
@@ -572,7 +575,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="29.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="25.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="24.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
@@ -1295,7 +1298,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1326,7 +1329,7 @@
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>43</v>
@@ -1705,7 +1708,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1715,7 +1718,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0.000037755678904071</v>
@@ -1727,7 +1730,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0.0512509147426044</v>
@@ -1739,7 +1742,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>-0.000712762935743738</v>
@@ -1751,7 +1754,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>-0.00288714747448697</v>
@@ -1763,7 +1766,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>0.0279172999524435</v>
@@ -1775,7 +1778,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0.0762965577128866</v>
@@ -1795,7 +1798,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1805,23 +1808,23 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>0.0235654096607136</v>
@@ -1837,7 +1840,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0.205217999472642</v>
@@ -1853,7 +1856,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>52.5283986804054</v>
@@ -1869,7 +1872,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.0150607924155383</v>
@@ -1885,7 +1888,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>6.41004881367893</v>
@@ -1901,7 +1904,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>39.2429538124787</v>
@@ -1917,7 +1920,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>22.6600776407273</v>
@@ -1933,7 +1936,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>121.085323148839</v>
@@ -1955,7 +1958,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1965,7 +1968,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>40</v>
@@ -1981,7 +1984,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>3</v>
@@ -1997,7 +2000,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>99</v>
@@ -2013,7 +2016,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>297</v>
@@ -2037,7 +2040,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2047,7 +2050,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>40</v>
@@ -2067,7 +2070,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>1</v>
@@ -2087,7 +2090,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>99</v>
@@ -2107,7 +2110,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>99</v>

</xml_diff>